<commit_message>
Add one history of CNN reference
</commit_message>
<xml_diff>
--- a/References.xlsx
+++ b/References.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>Dumoulin, Vincent, and Francesco Visin. "A guide to convolution arithmetic for deep learning."</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>https://arxiv.org/pdf/1703.06870</t>
+  </si>
+  <si>
+    <t>https://blog.athelas.com/a-brief-history-of-cnns-in-image-segmentation-from-r-cnn-to-mask-r-cnn-34ea83205de4</t>
+  </si>
+  <si>
+    <t>Dhruv Parthasarathy, "A Brief History of CNNs in Image Segmentation: From R-CNN to Mask R-CNN"</t>
   </si>
 </sst>
 </file>
@@ -598,31 +604,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="3.3046875" style="7" customWidth="1"/>
     <col min="2" max="2" width="15" style="7" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.7109375" style="9" customWidth="1"/>
-    <col min="12" max="12" width="26.5703125" style="9" customWidth="1"/>
-    <col min="15" max="15" width="34.28515625" customWidth="1"/>
-    <col min="16" max="16" width="51.42578125" customWidth="1"/>
-    <col min="17" max="17" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.3828125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="20.69140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="4.69140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.84375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="33.84375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="23.84375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="4.3828125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="12.3046875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.69140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="26.53515625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="34.3046875" customWidth="1"/>
+    <col min="16" max="16" width="51.3828125" customWidth="1"/>
+    <col min="17" max="17" width="34.69140625" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -636,7 +642,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -671,7 +677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.4">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -697,7 +703,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -732,7 +738,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -767,7 +773,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -802,7 +808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -837,7 +843,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -863,7 +869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -892,7 +898,16 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="I10" s="7">
         <v>9</v>
       </c>
@@ -906,7 +921,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I11" s="7">
         <v>10</v>
       </c>
@@ -935,8 +950,9 @@
     <hyperlink ref="L5" r:id="rId20"/>
     <hyperlink ref="L9" r:id="rId21"/>
     <hyperlink ref="L10" r:id="rId22"/>
+    <hyperlink ref="D10" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>